<commit_message>
Xbox Controller Broadcasting to multiple robots or clients...essentially pub/sub
</commit_message>
<xml_diff>
--- a/Util/test2.xlsx
+++ b/Util/test2.xlsx
@@ -485,13 +485,13 @@
   <sheetData>
     <row r="6" spans="1:4">
       <c r="B6" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -499,13 +499,13 @@
         <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
         <v>3</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -513,13 +513,13 @@
         <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -527,13 +527,13 @@
         <v>2</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
         <v>3</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -541,13 +541,13 @@
         <v>3</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed path references to relative paths
</commit_message>
<xml_diff>
--- a/Util/test2.xlsx
+++ b/Util/test2.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet11" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet11" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -485,27 +485,27 @@
   <sheetData>
     <row r="6" spans="1:4">
       <c r="B6" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="B7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" t="s">
         <v>3</v>
       </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -513,27 +513,27 @@
         <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" t="s">
         <v>3</v>
       </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -541,13 +541,13 @@
         <v>3</v>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>